<commit_message>
Update New Results ( 21 files).xlsx
labels added to the DS
</commit_message>
<xml_diff>
--- a/New Results ( 21 files).xlsx
+++ b/New Results ( 21 files).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nojou\Documents\GitHub\SDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60E8F5F-096C-4F57-BA2F-301A2BBE2A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE92814C-AB82-42D6-8F39-79E9F6A839C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="10536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -723,9 +723,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -734,19 +746,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -866,6 +866,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'AVG graphs '!$B$3:$D$3</c:f>
@@ -887,7 +945,7 @@
             <c:numRef>
               <c:f>'AVG graphs '!$B$4:$D$4</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.66816438095238084</c:v>
@@ -931,6 +989,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'AVG graphs '!$B$3:$D$3</c:f>
@@ -952,7 +1068,7 @@
             <c:numRef>
               <c:f>'AVG graphs '!$B$5:$D$5</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.82586771428571415</c:v>
@@ -996,6 +1112,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'AVG graphs '!$B$3:$D$3</c:f>
@@ -1017,7 +1191,7 @@
             <c:numRef>
               <c:f>'AVG graphs '!$B$6:$D$6</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.83790328571428574</c:v>
@@ -1038,8 +1212,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1122,7 +1297,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1347,6 +1522,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'AVG graphs '!$B$16:$D$16</c:f>
@@ -1368,7 +1601,7 @@
             <c:numRef>
               <c:f>'AVG graphs '!$B$17:$D$17</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.77545633333333341</c:v>
@@ -1412,6 +1645,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'AVG graphs '!$B$16:$D$16</c:f>
@@ -1433,7 +1724,7 @@
             <c:numRef>
               <c:f>'AVG graphs '!$B$18:$D$18</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.76285642857142866</c:v>
@@ -1477,6 +1768,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'AVG graphs '!$B$16:$D$16</c:f>
@@ -1498,7 +1847,7 @@
             <c:numRef>
               <c:f>'AVG graphs '!$B$19:$D$19</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.74283266666666681</c:v>
@@ -1519,8 +1868,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1603,7 +1953,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1821,6 +2171,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'AVG graphs '!$B$27:$D$27</c:f>
@@ -1842,7 +2250,7 @@
             <c:numRef>
               <c:f>'AVG graphs '!$B$28:$D$28</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.66816438095238084</c:v>
@@ -1886,6 +2294,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'AVG graphs '!$B$27:$D$27</c:f>
@@ -1907,7 +2373,7 @@
             <c:numRef>
               <c:f>'AVG graphs '!$B$29:$D$29</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.82729628571428548</c:v>
@@ -1951,6 +2417,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'AVG graphs '!$B$27:$D$27</c:f>
@@ -1972,7 +2496,7 @@
             <c:numRef>
               <c:f>'AVG graphs '!$B$30:$D$30</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.83790328571428574</c:v>
@@ -1993,8 +2517,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2077,7 +2602,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2295,6 +2820,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'AVG graphs '!$B$42:$D$42</c:f>
@@ -2316,7 +2899,7 @@
             <c:numRef>
               <c:f>'AVG graphs '!$B$43:$D$43</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.70284976190476178</c:v>
@@ -2360,6 +2943,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'AVG graphs '!$B$42:$D$42</c:f>
@@ -2381,7 +3022,7 @@
             <c:numRef>
               <c:f>'AVG graphs '!$B$44:$D$44</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.79322309523809509</c:v>
@@ -2425,6 +3066,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'AVG graphs '!$B$42:$D$42</c:f>
@@ -2446,7 +3145,7 @@
             <c:numRef>
               <c:f>'AVG graphs '!$B$45:$D$45</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.78644366666666665</c:v>
@@ -2467,8 +3166,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2551,7 +3251,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4851,8 +5551,8 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>321944</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -4887,8 +5587,8 @@
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -4923,8 +5623,8 @@
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
@@ -4959,8 +5659,8 @@
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>112394</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
@@ -5191,7 +5891,7 @@
   <dimension ref="A2:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+      <selection activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
@@ -5201,12 +5901,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
-      <c r="A2" s="58"/>
-      <c r="B2" s="58" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
@@ -5223,13 +5923,13 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="56">
+      <c r="B4" s="69">
         <v>0.66816438095238084</v>
       </c>
-      <c r="C4" s="56">
+      <c r="C4" s="69">
         <v>0.83264242857142867</v>
       </c>
-      <c r="D4" s="56">
+      <c r="D4" s="69">
         <v>0.84732857142857143</v>
       </c>
     </row>
@@ -5237,13 +5937,13 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="56">
+      <c r="B5" s="69">
         <v>0.82586771428571415</v>
       </c>
-      <c r="C5" s="56">
+      <c r="C5" s="69">
         <v>0.84934714285714297</v>
       </c>
-      <c r="D5" s="56">
+      <c r="D5" s="69">
         <v>0.85808957142857145</v>
       </c>
     </row>
@@ -5251,23 +5951,23 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="69">
         <v>0.83790328571428574</v>
       </c>
-      <c r="C6" s="56">
+      <c r="C6" s="69">
         <v>0.84208323809523811</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="69">
         <v>0.84544404761904757</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="58"/>
-      <c r="B15" s="58" t="s">
+      <c r="A15" s="57"/>
+      <c r="B15" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
     </row>
     <row r="16" spans="1:4">
       <c r="B16" t="s">
@@ -5284,13 +5984,13 @@
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="56">
+      <c r="B17" s="69">
         <v>0.77545633333333341</v>
       </c>
-      <c r="C17" s="56">
+      <c r="C17" s="69">
         <v>0.81197861904761903</v>
       </c>
-      <c r="D17" s="56">
+      <c r="D17" s="69">
         <v>0.81969247619047603</v>
       </c>
     </row>
@@ -5298,13 +5998,13 @@
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="56">
+      <c r="B18" s="69">
         <v>0.76285642857142866</v>
       </c>
-      <c r="C18" s="56">
+      <c r="C18" s="69">
         <v>0.8184825238095238</v>
       </c>
-      <c r="D18" s="56">
+      <c r="D18" s="69">
         <v>0.83867480952380957</v>
       </c>
     </row>
@@ -5312,23 +6012,23 @@
       <c r="A19" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="56">
+      <c r="B19" s="69">
         <v>0.74283266666666681</v>
       </c>
-      <c r="C19" s="56">
+      <c r="C19" s="69">
         <v>0.78167999999999993</v>
       </c>
-      <c r="D19" s="56">
+      <c r="D19" s="69">
         <v>0.80609452380952396</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="58"/>
-      <c r="B26" s="58" t="s">
+      <c r="A26" s="57"/>
+      <c r="B26" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
     </row>
     <row r="27" spans="1:4">
       <c r="B27" t="s">
@@ -5345,13 +6045,13 @@
       <c r="A28" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="56">
+      <c r="B28" s="69">
         <v>0.66816438095238084</v>
       </c>
-      <c r="C28" s="56">
+      <c r="C28" s="69">
         <v>0.83264242857142867</v>
       </c>
-      <c r="D28" s="56">
+      <c r="D28" s="69">
         <v>0.84732857142857143</v>
       </c>
     </row>
@@ -5359,13 +6059,13 @@
       <c r="A29" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="56">
+      <c r="B29" s="69">
         <v>0.82729628571428548</v>
       </c>
-      <c r="C29" s="56">
+      <c r="C29" s="69">
         <v>0.85077571428571441</v>
       </c>
-      <c r="D29" s="56">
+      <c r="D29" s="69">
         <v>0.85808957142857145</v>
       </c>
     </row>
@@ -5373,23 +6073,23 @@
       <c r="A30" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="56">
+      <c r="B30" s="69">
         <v>0.83790328571428574</v>
       </c>
-      <c r="C30" s="56">
+      <c r="C30" s="69">
         <v>0.84208323809523811</v>
       </c>
-      <c r="D30" s="56">
+      <c r="D30" s="69">
         <v>0.84544404761904757</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="58"/>
-      <c r="B41" s="58" t="s">
+      <c r="A41" s="57"/>
+      <c r="B41" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
     </row>
     <row r="42" spans="1:4">
       <c r="B42" t="s">
@@ -5406,13 +6106,13 @@
       <c r="A43" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="56">
+      <c r="B43" s="69">
         <v>0.70284976190476178</v>
       </c>
-      <c r="C43" s="56">
+      <c r="C43" s="69">
         <v>0.82161452380952382</v>
       </c>
-      <c r="D43" s="56">
+      <c r="D43" s="69">
         <v>0.83236861904761905</v>
       </c>
     </row>
@@ -5420,13 +6120,13 @@
       <c r="A44" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="56">
+      <c r="B44" s="69">
         <v>0.79322309523809509</v>
       </c>
-      <c r="C44" s="56">
+      <c r="C44" s="69">
         <v>0.83377000000000001</v>
       </c>
-      <c r="D44" s="56">
+      <c r="D44" s="69">
         <v>0.84775819047619039</v>
       </c>
     </row>
@@ -5434,13 +6134,13 @@
       <c r="A45" t="s">
         <v>3</v>
       </c>
-      <c r="B45" s="56">
+      <c r="B45" s="69">
         <v>0.78644366666666665</v>
       </c>
-      <c r="C45" s="56">
+      <c r="C45" s="69">
         <v>0.80867352380952384</v>
       </c>
-      <c r="D45" s="56">
+      <c r="D45" s="69">
         <v>0.82373209523809554</v>
       </c>
     </row>
@@ -5471,27 +6171,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="65" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="66"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="65" t="s">
+      <c r="F1" s="61"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="66"/>
-      <c r="J1" s="67"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="62"/>
     </row>
     <row r="2" spans="1:26" ht="16.8">
-      <c r="A2" s="69"/>
+      <c r="A2" s="59"/>
       <c r="B2" s="18" t="s">
         <v>4</v>
       </c>
@@ -5861,39 +6561,39 @@
         <v>28</v>
       </c>
       <c r="B13" s="48">
-        <f>AVERAGE(B3:B12)</f>
+        <f t="shared" ref="B13:J13" si="0">AVERAGE(B3:B12)</f>
         <v>0.65026059999999997</v>
       </c>
       <c r="C13" s="48">
-        <f>AVERAGE(C3:C12)</f>
+        <f t="shared" si="0"/>
         <v>0.80819569999999996</v>
       </c>
       <c r="D13" s="48">
-        <f>AVERAGE(D3:D12)</f>
+        <f t="shared" si="0"/>
         <v>0.81751839999999976</v>
       </c>
       <c r="E13" s="48">
-        <f>AVERAGE(E3:E12)</f>
+        <f t="shared" si="0"/>
         <v>0.78952639999999996</v>
       </c>
       <c r="F13" s="48">
-        <f>AVERAGE(F3:F12)</f>
+        <f t="shared" si="0"/>
         <v>0.81826870000000018</v>
       </c>
       <c r="G13" s="48">
-        <f>AVERAGE(G3:G12)</f>
+        <f t="shared" si="0"/>
         <v>0.82784780000000002</v>
       </c>
       <c r="H13" s="48">
-        <f>AVERAGE(H3:H12)</f>
+        <f t="shared" si="0"/>
         <v>0.76587059999999996</v>
       </c>
       <c r="I13" s="48">
-        <f>AVERAGE(I3:I12)</f>
+        <f t="shared" si="0"/>
         <v>0.77820320000000009</v>
       </c>
       <c r="J13" s="48">
-        <f>AVERAGE(J3:J12)</f>
+        <f t="shared" si="0"/>
         <v>0.81016670000000013</v>
       </c>
       <c r="K13" s="23"/>
@@ -6290,35 +6990,35 @@
         <v>0.75065809090909097</v>
       </c>
       <c r="C25" s="41">
-        <f t="shared" ref="C25:J25" si="0">AVERAGE(C14:C24)</f>
+        <f t="shared" ref="C25:J25" si="1">AVERAGE(C14:C24)</f>
         <v>0.83381345454545441</v>
       </c>
       <c r="D25" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.84586881818181814</v>
       </c>
       <c r="E25" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.7965837272727273</v>
       </c>
       <c r="F25" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.84786209090909104</v>
       </c>
       <c r="G25" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.86585854545454555</v>
       </c>
       <c r="H25" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80514645454545442</v>
       </c>
       <c r="I25" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.83637381818181822</v>
       </c>
       <c r="J25" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.83606427272727268</v>
       </c>
     </row>
@@ -6327,39 +7027,39 @@
         <v>31</v>
       </c>
       <c r="B26" s="52">
-        <f>AVERAGE(B3:B12,B14:B24)</f>
+        <f t="shared" ref="B26:J26" si="2">AVERAGE(B3:B12,B14:B24)</f>
         <v>0.70284976190476178</v>
       </c>
       <c r="C26" s="52">
-        <f>AVERAGE(C3:C12,C14:C24)</f>
+        <f t="shared" si="2"/>
         <v>0.82161452380952382</v>
       </c>
       <c r="D26" s="52">
-        <f>AVERAGE(D3:D12,D14:D24)</f>
+        <f t="shared" si="2"/>
         <v>0.83236861904761905</v>
       </c>
       <c r="E26" s="52">
-        <f>AVERAGE(E3:E12,E14:E24)</f>
+        <f t="shared" si="2"/>
         <v>0.79322309523809509</v>
       </c>
       <c r="F26" s="52">
-        <f>AVERAGE(F3:F12,F14:F24)</f>
+        <f t="shared" si="2"/>
         <v>0.83377000000000001</v>
       </c>
       <c r="G26" s="52">
-        <f>AVERAGE(G3:G12,G14:G24)</f>
+        <f t="shared" si="2"/>
         <v>0.84775819047619039</v>
       </c>
       <c r="H26" s="52">
-        <f>AVERAGE(H3:H12,H14:H24)</f>
+        <f t="shared" si="2"/>
         <v>0.78644366666666665</v>
       </c>
       <c r="I26" s="52">
-        <f>AVERAGE(I3:I12,I14:I24)</f>
+        <f t="shared" si="2"/>
         <v>0.80867352380952384</v>
       </c>
       <c r="J26" s="52">
-        <f>AVERAGE(J3:J12,J14:J24)</f>
+        <f t="shared" si="2"/>
         <v>0.82373209523809554</v>
       </c>
     </row>
@@ -6382,7 +7082,7 @@
   <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26:J26"/>
+      <selection activeCell="A3" sqref="A3:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -6391,21 +7091,21 @@
       <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="65" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="66"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="65" t="s">
+      <c r="F1" s="61"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="66"/>
-      <c r="J1" s="67"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="62"/>
     </row>
     <row r="2" spans="1:26" ht="16.8">
       <c r="A2" s="64"/>
@@ -6778,39 +7478,39 @@
         <v>28</v>
       </c>
       <c r="B13" s="38">
-        <f>AVERAGE(B3:B12)</f>
+        <f t="shared" ref="B13:J13" si="0">AVERAGE(B3:B12)</f>
         <v>0.60075280000000009</v>
       </c>
       <c r="C13" s="38">
-        <f>AVERAGE(C3:C12)</f>
+        <f t="shared" si="0"/>
         <v>0.82460270000000002</v>
       </c>
       <c r="D13" s="38">
-        <f>AVERAGE(D3:D12)</f>
+        <f t="shared" si="0"/>
         <v>0.84192110000000009</v>
       </c>
       <c r="E13" s="38">
-        <f>AVERAGE(E3:E12)</f>
+        <f t="shared" si="0"/>
         <v>0.82817519999999989</v>
       </c>
       <c r="F13" s="38">
-        <f>AVERAGE(F3:F12)</f>
+        <f t="shared" si="0"/>
         <v>0.84521190000000002</v>
       </c>
       <c r="G13" s="38">
-        <f>AVERAGE(G3:G12)</f>
+        <f t="shared" si="0"/>
         <v>0.84912729999999992</v>
       </c>
       <c r="H13" s="38">
-        <f>AVERAGE(H3:H12)</f>
+        <f t="shared" si="0"/>
         <v>0.82689630000000014</v>
       </c>
       <c r="I13" s="38">
-        <f>AVERAGE(I3:I12)</f>
+        <f t="shared" si="0"/>
         <v>0.83226650000000002</v>
       </c>
       <c r="J13" s="38">
-        <f>AVERAGE(J3:J12)</f>
+        <f t="shared" si="0"/>
         <v>0.84093439999999986</v>
       </c>
       <c r="K13" s="10"/>
@@ -7207,35 +7907,35 @@
         <v>0.7294476363636363</v>
       </c>
       <c r="C25" s="42">
-        <f t="shared" ref="C25:J25" si="0">AVERAGE(C14:C24)</f>
+        <f t="shared" ref="C25:J25" si="1">AVERAGE(C14:C24)</f>
         <v>0.83995127272727277</v>
       </c>
       <c r="D25" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.8522444545454545</v>
       </c>
       <c r="E25" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.82649727272727269</v>
       </c>
       <c r="F25" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.85583372727272722</v>
       </c>
       <c r="G25" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.86623709090909096</v>
       </c>
       <c r="H25" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.84790963636363648</v>
       </c>
       <c r="I25" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.85100754545454549</v>
       </c>
       <c r="J25" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.84954372727272731</v>
       </c>
     </row>
@@ -7244,39 +7944,39 @@
         <v>31</v>
       </c>
       <c r="B26" s="44">
-        <f>AVERAGE(B3:B12,B14:B24)</f>
+        <f t="shared" ref="B26:J26" si="2">AVERAGE(B3:B12,B14:B24)</f>
         <v>0.66816438095238084</v>
       </c>
       <c r="C26" s="44">
-        <f>AVERAGE(C3:C12,C14:C24)</f>
+        <f t="shared" si="2"/>
         <v>0.83264242857142867</v>
       </c>
       <c r="D26" s="44">
-        <f>AVERAGE(D3:D12,D14:D24)</f>
+        <f t="shared" si="2"/>
         <v>0.84732857142857143</v>
       </c>
       <c r="E26" s="44">
-        <f>AVERAGE(E3:E12,E14:E24)</f>
+        <f t="shared" si="2"/>
         <v>0.82729628571428548</v>
       </c>
       <c r="F26" s="44">
-        <f>AVERAGE(F3:F12,F14:F24)</f>
+        <f t="shared" si="2"/>
         <v>0.85077571428571441</v>
       </c>
       <c r="G26" s="44">
-        <f>AVERAGE(G3:G12,G14:G24)</f>
+        <f t="shared" si="2"/>
         <v>0.85808957142857145</v>
       </c>
       <c r="H26" s="44">
-        <f>AVERAGE(H3:H12,H14:H24)</f>
+        <f t="shared" si="2"/>
         <v>0.83790328571428574</v>
       </c>
       <c r="I26" s="44">
-        <f>AVERAGE(I3:I12,I14:I24)</f>
+        <f t="shared" si="2"/>
         <v>0.84208323809523811</v>
       </c>
       <c r="J26" s="44">
-        <f>AVERAGE(J3:J12,J14:J24)</f>
+        <f t="shared" si="2"/>
         <v>0.84544404761904757</v>
       </c>
     </row>
@@ -7308,21 +8008,21 @@
       <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="65" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="66"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="65" t="s">
+      <c r="F1" s="61"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="66"/>
-      <c r="J1" s="67"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="62"/>
     </row>
     <row r="2" spans="1:26" ht="16.8">
       <c r="A2" s="64"/>
@@ -7695,39 +8395,39 @@
         <v>28</v>
       </c>
       <c r="B13" s="45">
-        <f>AVERAGE(B3:B12)</f>
+        <f t="shared" ref="B13:J13" si="0">AVERAGE(B3:B12)</f>
         <v>0.74396369999999989</v>
       </c>
       <c r="C13" s="45">
-        <f>AVERAGE(C3:C12)</f>
+        <f t="shared" si="0"/>
         <v>0.79428440000000011</v>
       </c>
       <c r="D13" s="45">
-        <f>AVERAGE(D3:D12)</f>
+        <f t="shared" si="0"/>
         <v>0.79756450000000001</v>
       </c>
       <c r="E13" s="45">
-        <f>AVERAGE(E3:E12)</f>
+        <f t="shared" si="0"/>
         <v>0.75563499999999995</v>
       </c>
       <c r="F13" s="45">
-        <f>AVERAGE(F3:F12)</f>
+        <f t="shared" si="0"/>
         <v>0.79452689999999992</v>
       </c>
       <c r="G13" s="45">
-        <f>AVERAGE(G3:G12)</f>
+        <f t="shared" si="0"/>
         <v>0.80893050000000011</v>
       </c>
       <c r="H13" s="45">
-        <f>AVERAGE(H3:H12)</f>
+        <f t="shared" si="0"/>
         <v>0.71489479999999994</v>
       </c>
       <c r="I13" s="45">
-        <f>AVERAGE(I3:I12)</f>
+        <f t="shared" si="0"/>
         <v>0.73291679999999992</v>
       </c>
       <c r="J13" s="45">
-        <f>AVERAGE(J3:J12)</f>
+        <f t="shared" si="0"/>
         <v>0.78300100000000017</v>
       </c>
       <c r="K13" s="23"/>
@@ -8124,76 +8824,76 @@
         <v>0.80408599999999997</v>
       </c>
       <c r="C25" s="47">
-        <f t="shared" ref="C25:J25" si="0">AVERAGE(C14:C24)</f>
+        <f t="shared" ref="C25:J25" si="1">AVERAGE(C14:C24)</f>
         <v>0.82806427272727268</v>
       </c>
       <c r="D25" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.83980881818181818</v>
       </c>
       <c r="E25" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.7694213636363636</v>
       </c>
       <c r="F25" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.84026036363636358</v>
       </c>
       <c r="G25" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.86571509090909093</v>
       </c>
       <c r="H25" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.76823072727272745</v>
       </c>
       <c r="I25" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.82601018181818187</v>
       </c>
       <c r="J25" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.82708863636363639</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A26" s="57" t="s">
+      <c r="A26" s="56" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="53">
-        <f>AVERAGE(B3:B12,B14:B24)</f>
+        <f t="shared" ref="B26:J26" si="2">AVERAGE(B3:B12,B14:B24)</f>
         <v>0.77545633333333341</v>
       </c>
       <c r="C26" s="53">
-        <f>AVERAGE(C3:C12,C14:C24)</f>
+        <f t="shared" si="2"/>
         <v>0.81197861904761903</v>
       </c>
       <c r="D26" s="53">
-        <f>AVERAGE(D3:D12,D14:D24)</f>
+        <f t="shared" si="2"/>
         <v>0.81969247619047603</v>
       </c>
       <c r="E26" s="53">
-        <f>AVERAGE(E3:E12,E14:E24)</f>
+        <f t="shared" si="2"/>
         <v>0.76285642857142866</v>
       </c>
       <c r="F26" s="53">
-        <f>AVERAGE(F3:F12,F14:F24)</f>
+        <f t="shared" si="2"/>
         <v>0.8184825238095238</v>
       </c>
       <c r="G26" s="53">
-        <f>AVERAGE(G3:G12,G14:G24)</f>
+        <f t="shared" si="2"/>
         <v>0.83867480952380957</v>
       </c>
       <c r="H26" s="53">
-        <f>AVERAGE(H3:H12,H14:H24)</f>
+        <f t="shared" si="2"/>
         <v>0.74283266666666681</v>
       </c>
       <c r="I26" s="53">
-        <f>AVERAGE(I3:I12,I14:I24)</f>
+        <f t="shared" si="2"/>
         <v>0.78167999999999993</v>
       </c>
       <c r="J26" s="53">
-        <f>AVERAGE(J3:J12,J14:J24)</f>
+        <f t="shared" si="2"/>
         <v>0.80609452380952396</v>
       </c>
     </row>
@@ -8228,27 +8928,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="29.05" customHeight="1" thickBot="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="61" t="s">
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="61" t="s">
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
     </row>
     <row r="2" spans="1:26" ht="17.100000000000001" thickTop="1" thickBot="1">
-      <c r="A2" s="60"/>
+      <c r="A2" s="66"/>
       <c r="B2" s="20" t="s">
         <v>4</v>
       </c>
@@ -8618,39 +9318,39 @@
         <v>28</v>
       </c>
       <c r="B13" s="37">
-        <f>AVERAGE(B3:B12)</f>
+        <f t="shared" ref="B13:J13" si="0">AVERAGE(B3:B12)</f>
         <v>0.60075280000000009</v>
       </c>
       <c r="C13" s="38">
-        <f>AVERAGE(C3:C12)</f>
+        <f t="shared" si="0"/>
         <v>0.82460270000000002</v>
       </c>
       <c r="D13" s="39">
-        <f>AVERAGE(D3:D12)</f>
+        <f t="shared" si="0"/>
         <v>0.84192110000000009</v>
       </c>
       <c r="E13" s="38">
-        <f>AVERAGE(E3:E12)</f>
+        <f t="shared" si="0"/>
         <v>0.82817519999999989</v>
       </c>
       <c r="F13" s="38">
-        <f>AVERAGE(F3:F12)</f>
+        <f t="shared" si="0"/>
         <v>0.84521190000000002</v>
       </c>
       <c r="G13" s="39">
-        <f>AVERAGE(G3:G12)</f>
+        <f t="shared" si="0"/>
         <v>0.84912729999999992</v>
       </c>
       <c r="H13" s="38">
-        <f>AVERAGE(H3:H12)</f>
+        <f t="shared" si="0"/>
         <v>0.82689630000000014</v>
       </c>
       <c r="I13" s="38">
-        <f>AVERAGE(I3:I12)</f>
+        <f t="shared" si="0"/>
         <v>0.83226650000000002</v>
       </c>
       <c r="J13" s="39">
-        <f>AVERAGE(J3:J12)</f>
+        <f t="shared" si="0"/>
         <v>0.84093439999999986</v>
       </c>
       <c r="K13" s="10"/>
@@ -9047,35 +9747,35 @@
         <v>0.7294476363636363</v>
       </c>
       <c r="C25" s="42">
-        <f t="shared" ref="C25:J25" si="0">AVERAGE(C14:C24)</f>
+        <f t="shared" ref="C25:J25" si="1">AVERAGE(C14:C24)</f>
         <v>0.83995127272727277</v>
       </c>
       <c r="D25" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.8522444545454545</v>
       </c>
       <c r="E25" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.82377</v>
       </c>
       <c r="F25" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.85310645454545453</v>
       </c>
       <c r="G25" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.86623709090909096</v>
       </c>
       <c r="H25" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.84790963636363648</v>
       </c>
       <c r="I25" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.85100754545454549</v>
       </c>
       <c r="J25" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.84954372727272731</v>
       </c>
     </row>
@@ -9084,39 +9784,39 @@
         <v>30</v>
       </c>
       <c r="B26" s="52">
-        <f>AVERAGE(B3:B12,B14:B24)</f>
+        <f t="shared" ref="B26:J26" si="2">AVERAGE(B3:B12,B14:B24)</f>
         <v>0.66816438095238084</v>
       </c>
       <c r="C26" s="53">
-        <f>AVERAGE(C3:C12,C14:C24)</f>
+        <f t="shared" si="2"/>
         <v>0.83264242857142867</v>
       </c>
       <c r="D26" s="54">
-        <f>AVERAGE(D3:D12,D14:D24)</f>
+        <f t="shared" si="2"/>
         <v>0.84732857142857143</v>
       </c>
       <c r="E26" s="53">
-        <f>AVERAGE(E3:E12,E14:E24)</f>
+        <f t="shared" si="2"/>
         <v>0.82586771428571415</v>
       </c>
       <c r="F26" s="53">
-        <f>AVERAGE(F3:F12,F14:F24)</f>
+        <f t="shared" si="2"/>
         <v>0.84934714285714297</v>
       </c>
       <c r="G26" s="54">
-        <f>AVERAGE(G3:G12,G14:G24)</f>
+        <f t="shared" si="2"/>
         <v>0.85808957142857145</v>
       </c>
       <c r="H26" s="53">
-        <f>AVERAGE(H3:H12,H14:H24)</f>
+        <f t="shared" si="2"/>
         <v>0.83790328571428574</v>
       </c>
       <c r="I26" s="53">
-        <f>AVERAGE(I3:I12,I14:I24)</f>
+        <f t="shared" si="2"/>
         <v>0.84208323809523811</v>
       </c>
       <c r="J26" s="54">
-        <f>AVERAGE(J3:J12,J14:J24)</f>
+        <f t="shared" si="2"/>
         <v>0.84544404761904757</v>
       </c>
     </row>

</xml_diff>